<commit_message>
Final reclassification of 20000 sample records
</commit_message>
<xml_diff>
--- a/classification_timing.xlsx
+++ b/classification_timing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41d509ce3db0a387/GitHub/seattle-service-requests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{63D7FA29-4518-4098-AB30-6C9C7986FCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7D2D4F93-3FCB-4FB2-8BCE-D19D48E9071B}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{63D7FA29-4518-4098-AB30-6C9C7986FCEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F31FD5E3-8065-4BD0-8E78-1EEDD913403A}"/>
   <bookViews>
-    <workbookView xWindow="8685" yWindow="2265" windowWidth="20205" windowHeight="12945" xr2:uid="{FBBBC43A-F6D5-48C5-A8CF-2F6E6C69AC29}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{FBBBC43A-F6D5-48C5-A8CF-2F6E6C69AC29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Sample</t>
   </si>
   <si>
     <t>Runtime</t>
+  </si>
+  <si>
+    <t>FindIt-FixIt Reclassification Runtimes</t>
+  </si>
+  <si>
+    <t>Running on Azure VM:</t>
+  </si>
+  <si>
+    <t>Standard NV8as v4 (8 vcpus, 28 GiB memory, 0.25 GPU)</t>
   </si>
 </sst>
 </file>
@@ -111,6 +120,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Reclassification</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Runtime</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -151,7 +190,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$C$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -197,6 +236,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.4665457130358705"/>
+                  <c:y val="-2.287474482356372E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -229,10 +274,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:f>Sheet1!$B$6:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>20</c:v>
                 </c:pt>
@@ -252,56 +297,107 @@
                   <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1000</c:v>
+                  <c:v>999</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>749</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>649</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>599</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>699</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="35">
                   <c:v>500</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>750</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>650</c:v>
+                <c:pt idx="36">
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$21</c:f>
+              <c:f>Sheet1!$C$6:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="37"/>
                 <c:pt idx="0">
                   <c:v>1.19</c:v>
                 </c:pt>
@@ -361,6 +457,57 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>92.32</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200.61</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>66.8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>135.51</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>105.92</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>132.19</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>102.08</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>123.14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>64.150000000000006</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>146.96</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>94.34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>124.81</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>195.28</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>142.25</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>119.69</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>51.07</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>119.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -368,7 +515,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-74D9-4360-916B-1EF42888C1DF}"/>
+              <c16:uniqueId val="{00000000-665D-48C0-95CE-5ABFAE782EDC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -380,11 +527,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="831490664"/>
-        <c:axId val="831491720"/>
+        <c:axId val="545561960"/>
+        <c:axId val="514837424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="831490664"/>
+        <c:axId val="545561960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,17 +540,72 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Text</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Verbatims</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -441,12 +643,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="831491720"/>
+        <c:crossAx val="514837424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="831491720"/>
+        <c:axId val="514837424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -455,17 +657,72 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -503,7 +760,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="831490664"/>
+        <c:crossAx val="545561960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1119,23 +1376,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>102393</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>140493</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{963C4785-4F4C-A838-B7E1-8B2749422118}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC5855EA-F49B-D770-B4A9-3900BE845D55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1154,6 +1411,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1473,180 +1734,329 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A2F9F0-F0FA-4EB4-A3A2-CF42CCA68907}">
-  <dimension ref="B1:C21"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B6">
         <v>20</v>
       </c>
-      <c r="C2">
+      <c r="C6">
         <v>1.19</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B7">
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="C7">
         <v>17.41</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B8">
         <v>200</v>
       </c>
-      <c r="C4">
+      <c r="C8">
         <v>32.479999999999997</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5">
-        <v>500</v>
-      </c>
-      <c r="C5">
-        <v>79.45</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6">
-        <v>222.19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7">
-        <v>1000</v>
-      </c>
-      <c r="C7">
-        <v>167.88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B8">
-        <v>1000</v>
-      </c>
-      <c r="C8">
-        <v>200.69</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>500</v>
       </c>
       <c r="C9">
+        <v>79.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>1000</v>
+      </c>
+      <c r="C10">
+        <v>222.19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B11">
+        <v>1000</v>
+      </c>
+      <c r="C11">
+        <v>167.88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B12">
+        <v>999</v>
+      </c>
+      <c r="C12">
+        <v>200.69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B13">
+        <v>499</v>
+      </c>
+      <c r="C13">
         <v>124.81</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B10">
-        <v>500</v>
-      </c>
-      <c r="C10">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>499</v>
+      </c>
+      <c r="C14">
         <v>60.43</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B11">
-        <v>500</v>
-      </c>
-      <c r="C11">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>499</v>
+      </c>
+      <c r="C15">
         <v>142.09</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12">
-        <v>500</v>
-      </c>
-      <c r="C12">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B16">
+        <v>499</v>
+      </c>
+      <c r="C16">
         <v>141.53</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13">
-        <v>500</v>
-      </c>
-      <c r="C13">
-        <v>88.01</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14">
-        <v>500</v>
-      </c>
-      <c r="C14">
-        <v>73.05</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15">
-        <v>1000</v>
-      </c>
-      <c r="C15">
-        <v>193.77</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16">
-        <v>1000</v>
-      </c>
-      <c r="C16">
-        <v>115.58</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C17">
-        <v>66.459999999999994</v>
+        <v>88.01</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C18">
-        <v>123.64</v>
+        <v>73.05</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19">
-        <v>750</v>
+        <v>999</v>
       </c>
       <c r="C19">
-        <v>109.9</v>
+        <v>193.77</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20">
-        <v>600</v>
+        <v>999</v>
       </c>
       <c r="C20">
-        <v>167.38</v>
+        <v>115.58</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21">
-        <v>650</v>
+        <v>499</v>
       </c>
       <c r="C21">
+        <v>66.459999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <v>499</v>
+      </c>
+      <c r="C22">
+        <v>123.64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <v>749</v>
+      </c>
+      <c r="C23">
+        <v>109.9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <v>599</v>
+      </c>
+      <c r="C24">
+        <v>167.38</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <v>649</v>
+      </c>
+      <c r="C25">
         <v>92.32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <v>749</v>
+      </c>
+      <c r="C26">
+        <v>200.61</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>649</v>
+      </c>
+      <c r="C27">
+        <v>66.8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>499</v>
+      </c>
+      <c r="C28">
+        <v>135.51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>599</v>
+      </c>
+      <c r="C29">
+        <v>105.92</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>598</v>
+      </c>
+      <c r="C30">
+        <v>132.19</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>599</v>
+      </c>
+      <c r="C31">
+        <v>102.08</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B32">
+        <v>599</v>
+      </c>
+      <c r="C32">
+        <v>123.14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33">
+        <v>599</v>
+      </c>
+      <c r="C33">
+        <v>64.150000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>699</v>
+      </c>
+      <c r="C34">
+        <v>146.96</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35">
+        <v>699</v>
+      </c>
+      <c r="C35">
+        <v>94.34</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>699</v>
+      </c>
+      <c r="C36">
+        <v>124.81</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <v>699</v>
+      </c>
+      <c r="C37">
+        <v>195.28</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38">
+        <v>699</v>
+      </c>
+      <c r="C38">
+        <v>142.25</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39">
+        <v>699</v>
+      </c>
+      <c r="C39">
+        <v>119.69</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40">
+        <v>449</v>
+      </c>
+      <c r="C40">
+        <v>51.07</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41">
+        <v>500</v>
+      </c>
+      <c r="C41">
+        <v>119.4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42">
+        <v>80</v>
+      </c>
+      <c r="C42">
+        <v>6.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>